<commit_message>
Working on combining uses
</commit_message>
<xml_diff>
--- a/data/BuildingData.xlsx
+++ b/data/BuildingData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloud\Box\Sustainability and Utilities\Internal Strategy\Net Zero Carbon Pathways\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRode\OneDrive - Tishman Speyer\Documents\R\NCZ_Interventions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{126F0775-9B52-4941-9568-1122A845F7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DA82E6-6A85-45DD-B788-F6F8D5263426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="86">
   <si>
     <t>Building</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>San Diego</t>
+  </si>
+  <si>
+    <t>Note</t>
   </si>
 </sst>
 </file>
@@ -296,7 +299,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -778,7 +781,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1137,17 +1140,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1160,8 +1165,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1175,7 +1183,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1189,7 +1197,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1203,7 +1211,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1217,7 +1225,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1231,7 +1239,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1245,7 +1253,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1259,7 +1267,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1273,7 +1281,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1287,7 +1295,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1301,7 +1309,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1315,7 +1323,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1329,7 +1337,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1343,7 +1351,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1357,7 +1365,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1374,7 +1382,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1391,7 +1399,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1408,7 +1416,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1422,7 +1430,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1436,7 +1444,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1450,7 +1458,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1464,7 +1472,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1478,7 +1486,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1492,7 +1500,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1506,7 +1514,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1520,7 +1528,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1534,7 +1542,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1548,7 +1556,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1562,7 +1570,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1576,7 +1584,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1590,7 +1598,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1604,7 +1612,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1618,7 +1626,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1632,7 +1640,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1646,7 +1654,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1660,7 +1668,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1674,7 +1682,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1688,7 +1696,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1702,7 +1710,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -1716,7 +1724,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1730,7 +1738,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1744,7 +1752,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -1758,7 +1766,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1772,7 +1780,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1786,7 +1794,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -1800,7 +1808,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -1814,7 +1822,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1828,7 +1836,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1842,7 +1850,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1856,7 +1864,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1870,7 +1878,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1884,7 +1892,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -1898,7 +1906,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -1912,7 +1920,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -1926,7 +1934,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -1940,7 +1948,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -1954,7 +1962,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -1968,7 +1976,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -1982,7 +1990,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -1996,7 +2004,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -2010,7 +2018,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -2024,7 +2032,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -2038,7 +2046,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -2052,7 +2060,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -2066,7 +2074,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -2080,7 +2088,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -2094,7 +2102,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
Adding configurations by fuel
</commit_message>
<xml_diff>
--- a/data/BuildingData.xlsx
+++ b/data/BuildingData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRode\OneDrive - Tishman Speyer\Documents\R\NCZ_Interventions\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DA82E6-6A85-45DD-B788-F6F8D5263426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{86DA82E6-6A85-45DD-B788-F6F8D5263426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DCF6766-986C-473C-87E4-789249E80B4C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingData" sheetId="1" r:id="rId1"/>
+    <sheet name="Lists" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="95">
   <si>
     <t>Building</t>
   </si>
@@ -291,6 +292,33 @@
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>Primary Heating</t>
+  </si>
+  <si>
+    <t>DHW</t>
+  </si>
+  <si>
+    <t>Elect</t>
+  </si>
+  <si>
+    <t>Primary Cooling</t>
+  </si>
+  <si>
+    <t>NGas</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>Oil2</t>
+  </si>
+  <si>
+    <t>Oil4</t>
+  </si>
+  <si>
+    <t>Dielsel</t>
   </si>
 </sst>
 </file>
@@ -1138,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1150,9 +1178,10 @@
     <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1166,10 +1195,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1182,8 +1220,17 @@
       <c r="D2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1196,8 +1243,17 @@
       <c r="D3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1210,8 +1266,17 @@
       <c r="D4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1224,8 +1289,17 @@
       <c r="D5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1238,8 +1312,17 @@
       <c r="D6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1252,8 +1335,17 @@
       <c r="D7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1266,8 +1358,17 @@
       <c r="D8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1280,8 +1381,17 @@
       <c r="D9" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1294,8 +1404,17 @@
       <c r="D10" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1308,8 +1427,17 @@
       <c r="D11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1322,8 +1450,17 @@
       <c r="D12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1336,8 +1473,17 @@
       <c r="D13" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1350,8 +1496,17 @@
       <c r="D14" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1364,8 +1519,17 @@
       <c r="D15" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1379,10 +1543,19 @@
         <v>6</v>
       </c>
       <c r="E16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1396,10 +1569,19 @@
         <v>6</v>
       </c>
       <c r="E17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1413,10 +1595,19 @@
         <v>6</v>
       </c>
       <c r="E18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1429,8 +1620,17 @@
       <c r="D19" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1443,8 +1643,17 @@
       <c r="D20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1457,8 +1666,17 @@
       <c r="D21" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1471,8 +1689,17 @@
       <c r="D22" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E22" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1485,8 +1712,17 @@
       <c r="D23" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E23" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1499,8 +1735,17 @@
       <c r="D24" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1513,8 +1758,17 @@
       <c r="D25" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1527,8 +1781,17 @@
       <c r="D26" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1541,8 +1804,17 @@
       <c r="D27" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1555,8 +1827,17 @@
       <c r="D28" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1569,8 +1850,17 @@
       <c r="D29" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1583,8 +1873,17 @@
       <c r="D30" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1597,8 +1896,17 @@
       <c r="D31" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E31" t="s">
+        <v>88</v>
+      </c>
+      <c r="F31" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1611,8 +1919,17 @@
       <c r="D32" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E32" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1625,8 +1942,17 @@
       <c r="D33" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E33" t="s">
+        <v>88</v>
+      </c>
+      <c r="F33" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1639,8 +1965,17 @@
       <c r="D34" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E34" t="s">
+        <v>88</v>
+      </c>
+      <c r="F34" t="s">
+        <v>88</v>
+      </c>
+      <c r="G34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1653,8 +1988,17 @@
       <c r="D35" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E35" t="s">
+        <v>88</v>
+      </c>
+      <c r="F35" t="s">
+        <v>88</v>
+      </c>
+      <c r="G35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1667,8 +2011,17 @@
       <c r="D36" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E36" t="s">
+        <v>88</v>
+      </c>
+      <c r="F36" t="s">
+        <v>88</v>
+      </c>
+      <c r="G36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1681,8 +2034,17 @@
       <c r="D37" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E37" t="s">
+        <v>88</v>
+      </c>
+      <c r="F37" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1695,8 +2057,17 @@
       <c r="D38" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E38" t="s">
+        <v>88</v>
+      </c>
+      <c r="F38" t="s">
+        <v>88</v>
+      </c>
+      <c r="G38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1709,8 +2080,17 @@
       <c r="D39" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E39" t="s">
+        <v>88</v>
+      </c>
+      <c r="F39" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -1723,8 +2103,17 @@
       <c r="D40" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E40" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1737,8 +2126,17 @@
       <c r="D41" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1751,8 +2149,17 @@
       <c r="D42" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F42" t="s">
+        <v>88</v>
+      </c>
+      <c r="G42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -1765,8 +2172,17 @@
       <c r="D43" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E43" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1779,8 +2195,17 @@
       <c r="D44" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E44" t="s">
+        <v>88</v>
+      </c>
+      <c r="F44" t="s">
+        <v>88</v>
+      </c>
+      <c r="G44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1793,8 +2218,17 @@
       <c r="D45" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E45" t="s">
+        <v>88</v>
+      </c>
+      <c r="F45" t="s">
+        <v>88</v>
+      </c>
+      <c r="G45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -1807,8 +2241,17 @@
       <c r="D46" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E46" t="s">
+        <v>88</v>
+      </c>
+      <c r="F46" t="s">
+        <v>88</v>
+      </c>
+      <c r="G46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -1821,8 +2264,17 @@
       <c r="D47" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E47" t="s">
+        <v>88</v>
+      </c>
+      <c r="F47" t="s">
+        <v>88</v>
+      </c>
+      <c r="G47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1835,8 +2287,17 @@
       <c r="D48" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F48" t="s">
+        <v>88</v>
+      </c>
+      <c r="G48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1849,8 +2310,17 @@
       <c r="D49" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E49" t="s">
+        <v>88</v>
+      </c>
+      <c r="F49" t="s">
+        <v>88</v>
+      </c>
+      <c r="G49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1863,8 +2333,17 @@
       <c r="D50" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E50" t="s">
+        <v>88</v>
+      </c>
+      <c r="F50" t="s">
+        <v>88</v>
+      </c>
+      <c r="G50" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1877,8 +2356,17 @@
       <c r="D51" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E51" t="s">
+        <v>88</v>
+      </c>
+      <c r="F51" t="s">
+        <v>88</v>
+      </c>
+      <c r="G51" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1891,8 +2379,17 @@
       <c r="D52" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E52" t="s">
+        <v>88</v>
+      </c>
+      <c r="F52" t="s">
+        <v>88</v>
+      </c>
+      <c r="G52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -1905,8 +2402,17 @@
       <c r="D53" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E53" t="s">
+        <v>88</v>
+      </c>
+      <c r="F53" t="s">
+        <v>88</v>
+      </c>
+      <c r="G53" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -1919,8 +2425,17 @@
       <c r="D54" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E54" t="s">
+        <v>88</v>
+      </c>
+      <c r="F54" t="s">
+        <v>88</v>
+      </c>
+      <c r="G54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -1933,8 +2448,17 @@
       <c r="D55" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E55" t="s">
+        <v>88</v>
+      </c>
+      <c r="F55" t="s">
+        <v>88</v>
+      </c>
+      <c r="G55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -1947,8 +2471,17 @@
       <c r="D56" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E56" t="s">
+        <v>88</v>
+      </c>
+      <c r="F56" t="s">
+        <v>88</v>
+      </c>
+      <c r="G56" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -1961,8 +2494,17 @@
       <c r="D57" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E57" t="s">
+        <v>88</v>
+      </c>
+      <c r="F57" t="s">
+        <v>88</v>
+      </c>
+      <c r="G57" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -1975,8 +2517,17 @@
       <c r="D58" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E58" t="s">
+        <v>88</v>
+      </c>
+      <c r="F58" t="s">
+        <v>88</v>
+      </c>
+      <c r="G58" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -1989,8 +2540,17 @@
       <c r="D59" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E59" t="s">
+        <v>88</v>
+      </c>
+      <c r="F59" t="s">
+        <v>88</v>
+      </c>
+      <c r="G59" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -2003,8 +2563,17 @@
       <c r="D60" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E60" t="s">
+        <v>88</v>
+      </c>
+      <c r="F60" t="s">
+        <v>88</v>
+      </c>
+      <c r="G60" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -2017,8 +2586,17 @@
       <c r="D61" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E61" t="s">
+        <v>88</v>
+      </c>
+      <c r="F61" t="s">
+        <v>88</v>
+      </c>
+      <c r="G61" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -2031,8 +2609,17 @@
       <c r="D62" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E62" t="s">
+        <v>88</v>
+      </c>
+      <c r="F62" t="s">
+        <v>88</v>
+      </c>
+      <c r="G62" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -2045,8 +2632,17 @@
       <c r="D63" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E63" t="s">
+        <v>88</v>
+      </c>
+      <c r="F63" t="s">
+        <v>88</v>
+      </c>
+      <c r="G63" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -2059,8 +2655,17 @@
       <c r="D64" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E64" t="s">
+        <v>88</v>
+      </c>
+      <c r="F64" t="s">
+        <v>88</v>
+      </c>
+      <c r="G64" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -2073,8 +2678,17 @@
       <c r="D65" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E65" t="s">
+        <v>88</v>
+      </c>
+      <c r="F65" t="s">
+        <v>88</v>
+      </c>
+      <c r="G65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -2087,8 +2701,17 @@
       <c r="D66" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E66" t="s">
+        <v>88</v>
+      </c>
+      <c r="F66" t="s">
+        <v>88</v>
+      </c>
+      <c r="G66" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -2101,8 +2724,17 @@
       <c r="D67" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E67" t="s">
+        <v>88</v>
+      </c>
+      <c r="F67" t="s">
+        <v>88</v>
+      </c>
+      <c r="G67" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>72</v>
       </c>
@@ -2114,6 +2746,72 @@
       </c>
       <c r="D68" t="s">
         <v>84</v>
+      </c>
+      <c r="E68" t="s">
+        <v>88</v>
+      </c>
+      <c r="F68" t="s">
+        <v>88</v>
+      </c>
+      <c r="G68" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{83FD05DD-3227-4BA0-B7CE-FC89C8E42238}">
+          <x14:formula1>
+            <xm:f>Lists!$A$1:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:G68</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A84C9AD2-74B0-4995-9FFD-CFB54AF9A490}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wrking on load use logic.
</commit_message>
<xml_diff>
--- a/data/BuildingData.xlsx
+++ b/data/BuildingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{86DA82E6-6A85-45DD-B788-F6F8D5263426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DCF6766-986C-473C-87E4-789249E80B4C}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:1_{86DA82E6-6A85-45DD-B788-F6F8D5263426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0938535-FACA-4527-95B2-BB541AAF4A8A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -867,6 +867,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1168,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1244,13 +1248,13 @@
         <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F3" t="s">
         <v>88</v>
       </c>
       <c r="G3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -1267,13 +1271,13 @@
         <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
         <v>88</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -1313,13 +1317,13 @@
         <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F6" t="s">
         <v>88</v>
       </c>
       <c r="G6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1336,13 +1340,13 @@
         <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F7" t="s">
         <v>88</v>
       </c>
       <c r="G7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1359,13 +1363,13 @@
         <v>74</v>
       </c>
       <c r="E8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F8" t="s">
         <v>88</v>
       </c>
       <c r="G8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1382,13 +1386,13 @@
         <v>74</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F9" t="s">
         <v>88</v>
       </c>
       <c r="G9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1405,13 +1409,13 @@
         <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F10" t="s">
         <v>88</v>
       </c>
       <c r="G10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1428,13 +1432,13 @@
         <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
         <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1451,13 +1455,13 @@
         <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F12" t="s">
         <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1474,13 +1478,13 @@
         <v>74</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F13" t="s">
         <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1497,13 +1501,13 @@
         <v>74</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F14" t="s">
         <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1520,13 +1524,13 @@
         <v>77</v>
       </c>
       <c r="E15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F15" t="s">
         <v>88</v>
       </c>
       <c r="G15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1543,13 +1547,13 @@
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F16" t="s">
         <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H16" t="s">
         <v>78</v>
@@ -1569,13 +1573,13 @@
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F17" t="s">
         <v>88</v>
       </c>
       <c r="G17" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H17" t="s">
         <v>78</v>
@@ -1595,13 +1599,13 @@
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F18" t="s">
         <v>88</v>
       </c>
       <c r="G18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H18" t="s">
         <v>78</v>
@@ -1621,13 +1625,13 @@
         <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F19" t="s">
         <v>88</v>
       </c>
       <c r="G19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1644,13 +1648,13 @@
         <v>75</v>
       </c>
       <c r="E20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F20" t="s">
         <v>88</v>
       </c>
       <c r="G20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1667,13 +1671,13 @@
         <v>75</v>
       </c>
       <c r="E21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F21" t="s">
         <v>88</v>
       </c>
       <c r="G21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -1690,13 +1694,13 @@
         <v>75</v>
       </c>
       <c r="E22" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F22" t="s">
         <v>88</v>
       </c>
       <c r="G22" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1713,13 +1717,13 @@
         <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F23" t="s">
         <v>88</v>
       </c>
       <c r="G23" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1736,13 +1740,13 @@
         <v>75</v>
       </c>
       <c r="E24" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F24" t="s">
         <v>88</v>
       </c>
       <c r="G24" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1759,13 +1763,13 @@
         <v>75</v>
       </c>
       <c r="E25" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F25" t="s">
         <v>88</v>
       </c>
       <c r="G25" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -1782,13 +1786,13 @@
         <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F26" t="s">
         <v>88</v>
       </c>
       <c r="G26" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1805,13 +1809,13 @@
         <v>75</v>
       </c>
       <c r="E27" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F27" t="s">
         <v>88</v>
       </c>
       <c r="G27" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1851,13 +1855,13 @@
         <v>79</v>
       </c>
       <c r="E29" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F29" t="s">
         <v>88</v>
       </c>
       <c r="G29" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1874,13 +1878,13 @@
         <v>76</v>
       </c>
       <c r="E30" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F30" t="s">
         <v>88</v>
       </c>
       <c r="G30" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1897,13 +1901,13 @@
         <v>76</v>
       </c>
       <c r="E31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F31" t="s">
         <v>88</v>
       </c>
       <c r="G31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1920,13 +1924,13 @@
         <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F32" t="s">
         <v>88</v>
       </c>
       <c r="G32" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -1943,13 +1947,13 @@
         <v>76</v>
       </c>
       <c r="E33" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F33" t="s">
         <v>88</v>
       </c>
       <c r="G33" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -1966,13 +1970,13 @@
         <v>79</v>
       </c>
       <c r="E34" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F34" t="s">
         <v>88</v>
       </c>
       <c r="G34" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -1989,13 +1993,13 @@
         <v>79</v>
       </c>
       <c r="E35" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F35" t="s">
         <v>88</v>
       </c>
       <c r="G35" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -2012,13 +2016,13 @@
         <v>74</v>
       </c>
       <c r="E36" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F36" t="s">
         <v>88</v>
       </c>
       <c r="G36" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -2035,13 +2039,13 @@
         <v>76</v>
       </c>
       <c r="E37" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F37" t="s">
         <v>88</v>
       </c>
       <c r="G37" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -2104,13 +2108,13 @@
         <v>79</v>
       </c>
       <c r="E40" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F40" t="s">
         <v>88</v>
       </c>
       <c r="G40" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -2127,13 +2131,13 @@
         <v>74</v>
       </c>
       <c r="E41" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F41" t="s">
         <v>88</v>
       </c>
       <c r="G41" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -2150,13 +2154,13 @@
         <v>75</v>
       </c>
       <c r="E42" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F42" t="s">
         <v>88</v>
       </c>
       <c r="G42" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -2173,13 +2177,13 @@
         <v>74</v>
       </c>
       <c r="E43" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F43" t="s">
         <v>88</v>
       </c>
       <c r="G43" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -2196,13 +2200,13 @@
         <v>81</v>
       </c>
       <c r="E44" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F44" t="s">
         <v>88</v>
       </c>
       <c r="G44" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -2219,13 +2223,13 @@
         <v>81</v>
       </c>
       <c r="E45" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F45" t="s">
         <v>88</v>
       </c>
       <c r="G45" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -2242,13 +2246,13 @@
         <v>81</v>
       </c>
       <c r="E46" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F46" t="s">
         <v>88</v>
       </c>
       <c r="G46" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -2265,13 +2269,13 @@
         <v>74</v>
       </c>
       <c r="E47" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F47" t="s">
         <v>88</v>
       </c>
       <c r="G47" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -2288,13 +2292,13 @@
         <v>76</v>
       </c>
       <c r="E48" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F48" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G48" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -2311,13 +2315,13 @@
         <v>76</v>
       </c>
       <c r="E49" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F49" t="s">
         <v>88</v>
       </c>
       <c r="G49" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
@@ -2334,13 +2338,13 @@
         <v>82</v>
       </c>
       <c r="E50" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F50" t="s">
         <v>88</v>
       </c>
       <c r="G50" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -2357,13 +2361,13 @@
         <v>76</v>
       </c>
       <c r="E51" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F51" t="s">
         <v>88</v>
       </c>
       <c r="G51" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
@@ -2380,13 +2384,13 @@
         <v>76</v>
       </c>
       <c r="E52" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F52" t="s">
         <v>88</v>
       </c>
       <c r="G52" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
@@ -2403,13 +2407,13 @@
         <v>75</v>
       </c>
       <c r="E53" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F53" t="s">
         <v>88</v>
       </c>
       <c r="G53" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
@@ -2426,13 +2430,13 @@
         <v>82</v>
       </c>
       <c r="E54" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F54" t="s">
         <v>88</v>
       </c>
       <c r="G54" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
@@ -2449,13 +2453,13 @@
         <v>74</v>
       </c>
       <c r="E55" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F55" t="s">
         <v>88</v>
       </c>
       <c r="G55" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -2472,13 +2476,13 @@
         <v>76</v>
       </c>
       <c r="E56" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F56" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G56" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
@@ -2495,13 +2499,13 @@
         <v>79</v>
       </c>
       <c r="E57" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F57" t="s">
         <v>88</v>
       </c>
       <c r="G57" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
@@ -2518,13 +2522,13 @@
         <v>77</v>
       </c>
       <c r="E58" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F58" t="s">
         <v>88</v>
       </c>
       <c r="G58" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -2541,13 +2545,13 @@
         <v>77</v>
       </c>
       <c r="E59" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F59" t="s">
         <v>88</v>
       </c>
       <c r="G59" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
@@ -2564,13 +2568,13 @@
         <v>77</v>
       </c>
       <c r="E60" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F60" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G60" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -2587,13 +2591,13 @@
         <v>83</v>
       </c>
       <c r="E61" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F61" t="s">
         <v>88</v>
       </c>
       <c r="G61" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
@@ -2610,13 +2614,13 @@
         <v>83</v>
       </c>
       <c r="E62" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F62" t="s">
         <v>88</v>
       </c>
       <c r="G62" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -2633,13 +2637,13 @@
         <v>74</v>
       </c>
       <c r="E63" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F63" t="s">
         <v>88</v>
       </c>
       <c r="G63" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
@@ -2679,13 +2683,13 @@
         <v>76</v>
       </c>
       <c r="E65" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F65" t="s">
         <v>88</v>
       </c>
       <c r="G65" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -2702,13 +2706,13 @@
         <v>84</v>
       </c>
       <c r="E66" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F66" t="s">
         <v>88</v>
       </c>
       <c r="G66" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -2725,13 +2729,13 @@
         <v>84</v>
       </c>
       <c r="E67" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F67" t="s">
         <v>88</v>
       </c>
       <c r="G67" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -2748,13 +2752,13 @@
         <v>84</v>
       </c>
       <c r="E68" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F68" t="s">
         <v>88</v>
       </c>
       <c r="G68" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working the allocation problem
</commit_message>
<xml_diff>
--- a/data/BuildingData.xlsx
+++ b/data/BuildingData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{86DA82E6-6A85-45DD-B788-F6F8D5263426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2DD0B23-39CB-4AD4-B7AF-D795307C1ACB}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{86DA82E6-6A85-45DD-B788-F6F8D5263426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FEB639B-A190-4A1A-97FE-E78DDFAF9E30}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingData" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="96">
   <si>
     <t>Building</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>Primary DHW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generator </t>
   </si>
 </sst>
 </file>
@@ -1166,22 +1169,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:H68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1204,10 +1207,13 @@
         <v>94</v>
       </c>
       <c r="H1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1229,8 +1235,11 @@
       <c r="G2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1252,8 +1261,11 @@
       <c r="G3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1275,8 +1287,11 @@
       <c r="G4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1298,8 +1313,11 @@
       <c r="G5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1321,8 +1339,11 @@
       <c r="G6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1344,8 +1365,11 @@
       <c r="G7" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1367,8 +1391,11 @@
       <c r="G8" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1390,8 +1417,11 @@
       <c r="G9" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1413,8 +1443,11 @@
       <c r="G10" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1436,8 +1469,11 @@
       <c r="G11" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1459,8 +1495,11 @@
       <c r="G12" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1482,8 +1521,11 @@
       <c r="G13" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1505,8 +1547,11 @@
       <c r="G14" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1528,8 +1573,11 @@
       <c r="G15" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1552,10 +1600,13 @@
         <v>89</v>
       </c>
       <c r="H16" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1578,10 +1629,13 @@
         <v>89</v>
       </c>
       <c r="H17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1604,10 +1658,13 @@
         <v>89</v>
       </c>
       <c r="H18" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1629,8 +1686,11 @@
       <c r="G19" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1652,8 +1712,11 @@
       <c r="G20" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1675,8 +1738,11 @@
       <c r="G21" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1698,8 +1764,11 @@
       <c r="G22" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1721,8 +1790,11 @@
       <c r="G23" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1744,8 +1816,11 @@
       <c r="G24" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1767,8 +1842,11 @@
       <c r="G25" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1790,8 +1868,11 @@
       <c r="G26" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1813,8 +1894,11 @@
       <c r="G27" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1836,8 +1920,11 @@
       <c r="G28" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1859,8 +1946,11 @@
       <c r="G29" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1882,8 +1972,11 @@
       <c r="G30" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1905,8 +1998,11 @@
       <c r="G31" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1928,8 +2024,11 @@
       <c r="G32" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1951,8 +2050,11 @@
       <c r="G33" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1974,8 +2076,11 @@
       <c r="G34" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1997,8 +2102,11 @@
       <c r="G35" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2020,8 +2128,11 @@
       <c r="G36" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2043,8 +2154,11 @@
       <c r="G37" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -2066,8 +2180,11 @@
       <c r="G38" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -2089,8 +2206,11 @@
       <c r="G39" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -2112,8 +2232,11 @@
       <c r="G40" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2135,8 +2258,11 @@
       <c r="G41" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2158,8 +2284,11 @@
       <c r="G42" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -2181,8 +2310,11 @@
       <c r="G43" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -2204,8 +2336,11 @@
       <c r="G44" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -2227,8 +2362,11 @@
       <c r="G45" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -2250,8 +2388,11 @@
       <c r="G46" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -2273,8 +2414,11 @@
       <c r="G47" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -2296,8 +2440,11 @@
       <c r="G48" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -2319,8 +2466,11 @@
       <c r="G49" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -2342,8 +2492,11 @@
       <c r="G50" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -2365,8 +2518,11 @@
       <c r="G51" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -2388,8 +2544,11 @@
       <c r="G52" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -2411,8 +2570,11 @@
       <c r="G53" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -2434,8 +2596,11 @@
       <c r="G54" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -2457,8 +2622,11 @@
       <c r="G55" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -2480,8 +2648,11 @@
       <c r="G56" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -2503,8 +2674,11 @@
       <c r="G57" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -2526,8 +2700,11 @@
       <c r="G58" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -2549,8 +2726,11 @@
       <c r="G59" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -2572,8 +2752,11 @@
       <c r="G60" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -2595,8 +2778,11 @@
       <c r="G61" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -2618,8 +2804,11 @@
       <c r="G62" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -2641,8 +2830,11 @@
       <c r="G63" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -2664,8 +2856,11 @@
       <c r="G64" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -2687,8 +2882,11 @@
       <c r="G65" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -2710,8 +2908,11 @@
       <c r="G66" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -2733,8 +2934,11 @@
       <c r="G67" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>72</v>
       </c>
@@ -2755,6 +2959,9 @@
       </c>
       <c r="G68" t="s">
         <v>89</v>
+      </c>
+      <c r="H68" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2766,7 +2973,7 @@
           <x14:formula1>
             <xm:f>Lists!$A$1:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:G68</xm:sqref>
+          <xm:sqref>E2:H68</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2782,34 +2989,34 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
getting the oil gen right
</commit_message>
<xml_diff>
--- a/data/BuildingData.xlsx
+++ b/data/BuildingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{86DA82E6-6A85-45DD-B788-F6F8D5263426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FEB639B-A190-4A1A-97FE-E78DDFAF9E30}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{86DA82E6-6A85-45DD-B788-F6F8D5263426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54707728-BD01-4C1D-A914-9A8F81CA3466}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -870,6 +870,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1171,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:H68"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1921,7 +1925,7 @@
         <v>87</v>
       </c>
       <c r="H28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
working the end use allocaions for oil and generator fules
</commit_message>
<xml_diff>
--- a/data/BuildingData.xlsx
+++ b/data/BuildingData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{86DA82E6-6A85-45DD-B788-F6F8D5263426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54707728-BD01-4C1D-A914-9A8F81CA3466}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{86DA82E6-6A85-45DD-B788-F6F8D5263426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{518663E0-848F-4FA8-908D-DE3C8CF9244C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,11 @@
     <sheet name="BuildingData" sheetId="1" r:id="rId1"/>
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -48,55 +51,97 @@
     <t>CITY</t>
   </si>
   <si>
+    <t>Primary Heating</t>
+  </si>
+  <si>
+    <t>Primary Cooling</t>
+  </si>
+  <si>
+    <t>Primary DHW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generator </t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
     <t>10 and 30 South Wacker</t>
   </si>
   <si>
     <t>office</t>
   </si>
   <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Elect</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>10900 Wilshire</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>NGas</t>
+  </si>
+  <si>
+    <t>1099 New York Ave.</t>
+  </si>
+  <si>
+    <t>Washington, D.C.</t>
+  </si>
+  <si>
+    <t>11 West 42nd Street</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>1120 G Street, NW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11975 W Bluff Creek Drive </t>
+  </si>
+  <si>
+    <t>11985 W Bluff Creek Drive</t>
+  </si>
+  <si>
+    <t>11995 W Bluff Creek Drive</t>
+  </si>
+  <si>
+    <t>12005 W Bluff Creek Drive</t>
+  </si>
+  <si>
+    <t>1201 F St.</t>
+  </si>
+  <si>
+    <t>12015 W Bluff Creek Drive</t>
+  </si>
+  <si>
+    <t>12105 West Waterfront Drive</t>
+  </si>
+  <si>
+    <t>12126 West Waterfront Drive</t>
+  </si>
+  <si>
+    <t>125 High Street</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>1275 Crossman</t>
+  </si>
+  <si>
     <t>city</t>
   </si>
   <si>
-    <t>10900 Wilshire</t>
-  </si>
-  <si>
-    <t>1099 New York Ave.</t>
-  </si>
-  <si>
-    <t>11 West 42nd Street</t>
-  </si>
-  <si>
-    <t>1120 G Street, NW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11975 W Bluff Creek Drive </t>
-  </si>
-  <si>
-    <t>11985 W Bluff Creek Drive</t>
-  </si>
-  <si>
-    <t>11995 W Bluff Creek Drive</t>
-  </si>
-  <si>
-    <t>12005 W Bluff Creek Drive</t>
-  </si>
-  <si>
-    <t>1201 F St.</t>
-  </si>
-  <si>
-    <t>12015 W Bluff Creek Drive</t>
-  </si>
-  <si>
-    <t>12105 West Waterfront Drive</t>
-  </si>
-  <si>
-    <t>12126 West Waterfront Drive</t>
-  </si>
-  <si>
-    <t>125 High Street</t>
-  </si>
-  <si>
-    <t>1275 Crossman</t>
+    <t>Don't own anymore (Sunnyvale campus)</t>
   </si>
   <si>
     <t>1345 Crossman</t>
@@ -108,6 +153,9 @@
     <t>160 Spear</t>
   </si>
   <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
     <t>1717 Penn Ave.</t>
   </si>
   <si>
@@ -120,6 +168,9 @@
     <t>175 Varick</t>
   </si>
   <si>
+    <t>Oil4</t>
+  </si>
+  <si>
     <t xml:space="preserve">1775 Penn Ave. </t>
   </si>
   <si>
@@ -135,6 +186,9 @@
     <t>222 N LaSalle</t>
   </si>
   <si>
+    <t>Oil2</t>
+  </si>
+  <si>
     <t>222 Second Street</t>
   </si>
   <si>
@@ -150,6 +204,9 @@
     <t>300 Park</t>
   </si>
   <si>
+    <t>Steam</t>
+  </si>
+  <si>
     <t>333 Bush</t>
   </si>
   <si>
@@ -165,6 +222,9 @@
     <t>520 Pike Tower</t>
   </si>
   <si>
+    <t>Seattle</t>
+  </si>
+  <si>
     <t>525 W Monroe</t>
   </si>
   <si>
@@ -183,6 +243,9 @@
     <t>Bala I</t>
   </si>
   <si>
+    <t>Bala Cynwyd</t>
+  </si>
+  <si>
     <t>Bala II</t>
   </si>
   <si>
@@ -201,6 +264,9 @@
     <t>GAC</t>
   </si>
   <si>
+    <t>Stamford</t>
+  </si>
+  <si>
     <t>Hearst Tower</t>
   </si>
   <si>
@@ -234,6 +300,9 @@
     <t>Reston Crossing I</t>
   </si>
   <si>
+    <t>Reston</t>
+  </si>
+  <si>
     <t>Reston Crossing II</t>
   </si>
   <si>
@@ -249,79 +318,13 @@
     <t>Torrey Plaza (A)</t>
   </si>
   <si>
+    <t>San Diego</t>
+  </si>
+  <si>
     <t>Torrey Plaza (B)</t>
   </si>
   <si>
     <t>Torrey Plaza (C)</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Los Angeles</t>
-  </si>
-  <si>
-    <t>Washington, D.C.</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>Don't own anymore (Sunnyvale campus)</t>
-  </si>
-  <si>
-    <t>San Francisco</t>
-  </si>
-  <si>
-    <t>Seattle</t>
-  </si>
-  <si>
-    <t>Bala Cynwyd</t>
-  </si>
-  <si>
-    <t>Stamford</t>
-  </si>
-  <si>
-    <t>Reston</t>
-  </si>
-  <si>
-    <t>San Diego</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>Primary Heating</t>
-  </si>
-  <si>
-    <t>Elect</t>
-  </si>
-  <si>
-    <t>Primary Cooling</t>
-  </si>
-  <si>
-    <t>NGas</t>
-  </si>
-  <si>
-    <t>Steam</t>
-  </si>
-  <si>
-    <t>Oil2</t>
-  </si>
-  <si>
-    <t>Oil4</t>
-  </si>
-  <si>
-    <t>Dielsel</t>
-  </si>
-  <si>
-    <t>Primary DHW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generator </t>
   </si>
 </sst>
 </file>
@@ -332,7 +335,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -872,14 +875,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -917,7 +916,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1023,7 +1022,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1165,7 +1164,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1175,20 +1174,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="16.26953125" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1202,1770 +1201,1770 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>94</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
         <v>2879120.28</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>236087</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>180271</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>958862</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1">
         <v>135096</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
         <v>44756</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
         <v>42887</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1">
         <v>44657</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1">
         <v>36438</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1">
         <v>244653</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
         <v>36392</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1">
         <v>296319</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1">
         <v>129313</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1">
         <v>1486596</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
       <c r="I16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H17" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
       <c r="I17" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H18" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
       <c r="I18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C19" s="1">
         <v>303429</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1">
         <v>202183</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1">
         <v>268704</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C22" s="1">
         <v>167926</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C23" s="1">
         <v>176119</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="H23" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1">
         <v>157480</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H24" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1">
         <v>290069</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C26" s="1">
         <v>234278</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E26" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H26" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C27" s="1">
         <v>340507</v>
       </c>
       <c r="D27" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F27" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C28" s="1">
         <v>1018838</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="F28" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G28" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C29" s="1">
         <v>453000</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="E29" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F29" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C30" s="1">
         <v>595200</v>
       </c>
       <c r="D30" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E30" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C31" s="1">
         <v>659780</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1">
         <v>540627</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H32" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1">
         <v>777658</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="F33" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="H33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C34" s="1">
         <v>597694</v>
       </c>
       <c r="D34" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="E34" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F34" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H34" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C35" s="1">
         <v>138762</v>
       </c>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="E35" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F35" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G35" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H35" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C36" s="1">
         <v>163811</v>
       </c>
       <c r="D36" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E36" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F36" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C37" s="1">
         <v>1049000</v>
       </c>
       <c r="D37" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="F37" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="H37" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C38" s="1">
         <v>425829</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="E38" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="F38" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G38" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="H38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C39" s="1">
         <v>1028492</v>
       </c>
       <c r="D39" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="E39" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="F39" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="H39" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C40" s="1">
         <v>429572</v>
       </c>
       <c r="D40" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="E40" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F40" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G40" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H40" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C41" s="1">
         <v>202444</v>
       </c>
       <c r="D41" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E41" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F41" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G41" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H41" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C42" s="1">
         <v>115272</v>
       </c>
       <c r="D42" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E42" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F42" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G42" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H42" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C43" s="1">
         <v>147000</v>
       </c>
       <c r="D43" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E43" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F43" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G43" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H43" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C44" s="1">
         <v>400386</v>
       </c>
       <c r="D44" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E44" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F44" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H44" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C45" s="1">
         <v>290011</v>
       </c>
       <c r="D45" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E45" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F45" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G45" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H45" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C46" s="1">
         <v>394764</v>
       </c>
       <c r="D46" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E46" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F46" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G46" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H46" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C47" s="1">
         <v>132289</v>
       </c>
       <c r="D47" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E47" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F47" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G47" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H47" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C48" s="1">
         <v>770389</v>
       </c>
       <c r="D48" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E48" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="F48" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="G48" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="H48" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C49" s="1">
         <v>370758</v>
       </c>
       <c r="D49" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E49" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="F49" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G49" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="H49" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C50" s="1">
         <v>648000</v>
       </c>
       <c r="D50" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E50" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="F50" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G50" t="s">
-        <v>91</v>
+        <v>49</v>
       </c>
       <c r="H50" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C51" s="1">
         <v>839272</v>
       </c>
       <c r="D51" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E51" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="F51" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G51" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="H51" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C52" s="1">
         <v>106583</v>
       </c>
       <c r="D52" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F52" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H52" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C53" s="1">
         <v>1167626</v>
       </c>
       <c r="D53" t="s">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E53" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F53" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G53" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H53" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C54" s="1">
         <v>313882</v>
       </c>
       <c r="D54" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E54" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F54" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G54" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H54" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C55" s="1">
         <v>289542</v>
       </c>
       <c r="D55" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E55" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F55" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G55" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H55" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C56" s="1">
         <v>3091809</v>
       </c>
       <c r="D56" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E56" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="F56" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="G56" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="H56" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C57" s="1">
         <v>451725</v>
       </c>
       <c r="D57" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="E57" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="F57" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G57" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="H57" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C58" s="1">
         <v>501650</v>
       </c>
       <c r="D58" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="E58" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F58" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G58" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H58" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C59" s="1">
         <v>342090</v>
       </c>
       <c r="D59" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="E59" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F59" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G59" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H59" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C60" s="1">
         <v>1118355</v>
       </c>
       <c r="D60" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="E60" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="F60" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="G60" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="H60" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C61" s="1">
         <v>160938</v>
       </c>
       <c r="D61" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E61" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F61" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G61" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H61" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C62" s="1">
         <v>187255</v>
       </c>
       <c r="D62" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E62" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" t="s">
+        <v>16</v>
+      </c>
+      <c r="H62" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
         <v>89</v>
       </c>
-      <c r="F62" t="s">
-        <v>87</v>
-      </c>
-      <c r="G62" t="s">
-        <v>89</v>
-      </c>
-      <c r="H62" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>67</v>
-      </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C63" s="1">
         <v>110080</v>
       </c>
       <c r="D63" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="E63" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F63" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G63" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H63" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C64" s="1">
         <v>3117492</v>
       </c>
       <c r="D64" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="E64" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="F64" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G64" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="H64" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C65" s="1">
         <v>1188749</v>
       </c>
       <c r="D65" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="E65" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F65" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G65" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H65" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C66" s="1">
         <v>60253</v>
       </c>
       <c r="D66" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="E66" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F66" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G66" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H66" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C67" s="1">
         <v>89132</v>
       </c>
       <c r="D67" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="E67" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F67" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G67" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H67" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C68" s="1">
         <v>75450</v>
       </c>
       <c r="D68" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="E68" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F68" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="G68" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="H68" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2993,36 +2992,36 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
catchup on work computer
</commit_message>
<xml_diff>
--- a/data/BuildingData.xlsx
+++ b/data/BuildingData.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{86DA82E6-6A85-45DD-B788-F6F8D5263426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{518663E0-848F-4FA8-908D-DE3C8CF9244C}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="114_{201A3308-3694-437F-AA18-B55609DB1918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2E5F161-3FB0-423F-BCB4-587179D7821C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3456" yWindow="3456" windowWidth="20304" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingData" sheetId="1" r:id="rId1"/>
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BuildingData!$A$1:$I$68</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -335,7 +338,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,9 +879,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -916,7 +919,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1022,7 +1025,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1164,7 +1167,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1172,22 +1175,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1216,7 +1220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1242,7 +1246,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1268,7 +1272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1294,7 +1298,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1320,7 +1324,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1346,7 +1350,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1372,7 +1376,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1398,7 +1402,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1424,7 +1428,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1450,7 +1454,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1476,7 +1480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -1502,7 +1506,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1528,7 +1532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1554,7 +1558,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1580,7 +1584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1609,7 +1613,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1638,7 +1642,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1667,7 +1671,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1693,7 +1697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1719,7 +1723,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1745,7 +1749,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1771,7 +1775,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1797,7 +1801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1823,7 +1827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1849,7 +1853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -1875,7 +1879,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -1901,7 +1905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1927,7 +1931,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -1953,7 +1957,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -1979,7 +1983,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -2005,7 +2009,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -2031,7 +2035,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -2057,7 +2061,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>56</v>
       </c>
@@ -2083,7 +2087,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -2109,7 +2113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -2135,7 +2139,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -2161,7 +2165,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>60</v>
       </c>
@@ -2187,7 +2191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>62</v>
       </c>
@@ -2213,7 +2217,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -2239,7 +2243,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>64</v>
       </c>
@@ -2265,7 +2269,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>65</v>
       </c>
@@ -2291,7 +2295,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>66</v>
       </c>
@@ -2317,7 +2321,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>67</v>
       </c>
@@ -2343,7 +2347,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -2369,7 +2373,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -2395,7 +2399,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -2421,7 +2425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -2447,7 +2451,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>73</v>
       </c>
@@ -2473,7 +2477,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -2499,7 +2503,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -2525,7 +2529,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>77</v>
       </c>
@@ -2551,7 +2555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>78</v>
       </c>
@@ -2577,7 +2581,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>79</v>
       </c>
@@ -2603,7 +2607,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>80</v>
       </c>
@@ -2629,7 +2633,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>81</v>
       </c>
@@ -2655,7 +2659,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>82</v>
       </c>
@@ -2681,7 +2685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>83</v>
       </c>
@@ -2707,7 +2711,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>84</v>
       </c>
@@ -2733,7 +2737,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>85</v>
       </c>
@@ -2759,7 +2763,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -2785,7 +2789,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>88</v>
       </c>
@@ -2811,7 +2815,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>89</v>
       </c>
@@ -2837,7 +2841,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>90</v>
       </c>
@@ -2863,7 +2867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>91</v>
       </c>
@@ -2889,7 +2893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>92</v>
       </c>
@@ -2915,7 +2919,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>94</v>
       </c>
@@ -2941,7 +2945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>95</v>
       </c>
@@ -2968,6 +2972,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I68" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="12015 W Bluff Creek Drive"/>
+        <filter val="160 Spear"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -2992,34 +3004,34 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>

</xml_diff>